<commit_message>
Add learning records for 2025-03-03
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -367,1838 +367,1838 @@
   <sheetData>
     <row r="1" spans="1:1" customFormat="false">
       <c r="A1" s="0" t="str">
-        <v>2025-02-22</v>
+        <v>2025-03-02</v>
       </c>
     </row>
     <row r="2" spans="1:3" customFormat="false">
       <c r="A2" s="0" t="str">
-        <v>2025-02-23</v>
+        <v>2025-03-03</v>
       </c>
       <c r="B2" s="0" t="str">
-        <v>5.0</v>
+        <v>fawef</v>
       </c>
       <c r="C2" s="0" t="str">
-        <v>何もしていなかった</v>
+        <v>wef</v>
       </c>
     </row>
     <row r="3" spans="1:1" customFormat="false">
       <c r="A3" s="0" t="str">
-        <v>2025-02-24</v>
+        <v>2025-03-04</v>
       </c>
     </row>
     <row r="4" spans="1:1" customFormat="false">
       <c r="A4" s="0" t="str">
-        <v>2025-02-25</v>
+        <v>2025-03-05</v>
       </c>
     </row>
     <row r="5" spans="1:1" customFormat="false">
       <c r="A5" s="0" t="str">
-        <v>2025-02-26</v>
+        <v>2025-03-06</v>
       </c>
     </row>
     <row r="6" spans="1:1" customFormat="false">
       <c r="A6" s="0" t="str">
-        <v>2025-02-27</v>
+        <v>2025-03-07</v>
       </c>
     </row>
     <row r="7" spans="1:1" customFormat="false">
       <c r="A7" s="0" t="str">
-        <v>2025-02-28</v>
+        <v>2025-03-08</v>
       </c>
     </row>
     <row r="8" spans="1:1" customFormat="false">
       <c r="A8" s="0" t="str">
-        <v>2025-03-01</v>
+        <v>2025-03-09</v>
       </c>
     </row>
     <row r="9" spans="1:1" customFormat="false">
       <c r="A9" s="0" t="str">
-        <v>2025-03-02</v>
+        <v>2025-03-10</v>
       </c>
     </row>
     <row r="10" spans="1:1" customFormat="false">
       <c r="A10" s="0" t="str">
-        <v>2025-03-03</v>
+        <v>2025-03-11</v>
       </c>
     </row>
     <row r="11" spans="1:1" customFormat="false">
       <c r="A11" s="0" t="str">
-        <v>2025-03-04</v>
+        <v>2025-03-12</v>
       </c>
     </row>
     <row r="12" spans="1:1" customFormat="false">
       <c r="A12" s="0" t="str">
-        <v>2025-03-05</v>
+        <v>2025-03-13</v>
       </c>
     </row>
     <row r="13" spans="1:1" customFormat="false">
       <c r="A13" s="0" t="str">
-        <v>2025-03-06</v>
+        <v>2025-03-14</v>
       </c>
     </row>
     <row r="14" spans="1:1" customFormat="false">
       <c r="A14" s="0" t="str">
-        <v>2025-03-07</v>
+        <v>2025-03-15</v>
       </c>
     </row>
     <row r="15" spans="1:1" customFormat="false">
       <c r="A15" s="0" t="str">
-        <v>2025-03-08</v>
+        <v>2025-03-16</v>
       </c>
     </row>
     <row r="16" spans="1:1" customFormat="false">
       <c r="A16" s="0" t="str">
-        <v>2025-03-09</v>
+        <v>2025-03-17</v>
       </c>
     </row>
     <row r="17" spans="1:1" customFormat="false">
       <c r="A17" s="0" t="str">
-        <v>2025-03-10</v>
+        <v>2025-03-18</v>
       </c>
     </row>
     <row r="18" spans="1:1" customFormat="false">
       <c r="A18" s="0" t="str">
-        <v>2025-03-11</v>
+        <v>2025-03-19</v>
       </c>
     </row>
     <row r="19" spans="1:1" customFormat="false">
       <c r="A19" s="0" t="str">
-        <v>2025-03-12</v>
+        <v>2025-03-20</v>
       </c>
     </row>
     <row r="20" spans="1:1" customFormat="false">
       <c r="A20" s="0" t="str">
-        <v>2025-03-13</v>
+        <v>2025-03-21</v>
       </c>
     </row>
     <row r="21" spans="1:1" customFormat="false">
       <c r="A21" s="0" t="str">
-        <v>2025-03-14</v>
+        <v>2025-03-22</v>
       </c>
     </row>
     <row r="22" spans="1:1" customFormat="false">
       <c r="A22" s="0" t="str">
-        <v>2025-03-15</v>
+        <v>2025-03-23</v>
       </c>
     </row>
     <row r="23" spans="1:1" customFormat="false">
       <c r="A23" s="0" t="str">
-        <v>2025-03-16</v>
+        <v>2025-03-24</v>
       </c>
     </row>
     <row r="24" spans="1:1" customFormat="false">
       <c r="A24" s="0" t="str">
-        <v>2025-03-17</v>
+        <v>2025-03-25</v>
       </c>
     </row>
     <row r="25" spans="1:1" customFormat="false">
       <c r="A25" s="0" t="str">
-        <v>2025-03-18</v>
+        <v>2025-03-26</v>
       </c>
     </row>
     <row r="26" spans="1:1" customFormat="false">
       <c r="A26" s="0" t="str">
-        <v>2025-03-19</v>
+        <v>2025-03-27</v>
       </c>
     </row>
     <row r="27" spans="1:1" customFormat="false">
       <c r="A27" s="0" t="str">
-        <v>2025-03-20</v>
+        <v>2025-03-28</v>
       </c>
     </row>
     <row r="28" spans="1:1" customFormat="false">
       <c r="A28" s="0" t="str">
-        <v>2025-03-21</v>
+        <v>2025-03-29</v>
       </c>
     </row>
     <row r="29" spans="1:1" customFormat="false">
       <c r="A29" s="0" t="str">
-        <v>2025-03-22</v>
+        <v>2025-03-30</v>
       </c>
     </row>
     <row r="30" spans="1:1" customFormat="false">
       <c r="A30" s="0" t="str">
-        <v>2025-03-23</v>
+        <v>2025-03-31</v>
       </c>
     </row>
     <row r="31" spans="1:1" customFormat="false">
       <c r="A31" s="0" t="str">
-        <v>2025-03-24</v>
+        <v>2025-04-01</v>
       </c>
     </row>
     <row r="32" spans="1:1" customFormat="false">
       <c r="A32" s="0" t="str">
-        <v>2025-03-25</v>
+        <v>2025-04-02</v>
       </c>
     </row>
     <row r="33" spans="1:1" customFormat="false">
       <c r="A33" s="0" t="str">
-        <v>2025-03-26</v>
+        <v>2025-04-03</v>
       </c>
     </row>
     <row r="34" spans="1:1" customFormat="false">
       <c r="A34" s="0" t="str">
-        <v>2025-03-27</v>
+        <v>2025-04-04</v>
       </c>
     </row>
     <row r="35" spans="1:1" customFormat="false">
       <c r="A35" s="0" t="str">
-        <v>2025-03-28</v>
+        <v>2025-04-05</v>
       </c>
     </row>
     <row r="36" spans="1:1" customFormat="false">
       <c r="A36" s="0" t="str">
-        <v>2025-03-29</v>
+        <v>2025-04-06</v>
       </c>
     </row>
     <row r="37" spans="1:1" customFormat="false">
       <c r="A37" s="0" t="str">
-        <v>2025-03-30</v>
+        <v>2025-04-07</v>
       </c>
     </row>
     <row r="38" spans="1:1" customFormat="false">
       <c r="A38" s="0" t="str">
-        <v>2025-03-31</v>
+        <v>2025-04-08</v>
       </c>
     </row>
     <row r="39" spans="1:1" customFormat="false">
       <c r="A39" s="0" t="str">
-        <v>2025-04-01</v>
+        <v>2025-04-09</v>
       </c>
     </row>
     <row r="40" spans="1:1" customFormat="false">
       <c r="A40" s="0" t="str">
-        <v>2025-04-02</v>
+        <v>2025-04-10</v>
       </c>
     </row>
     <row r="41" spans="1:1" customFormat="false">
       <c r="A41" s="0" t="str">
-        <v>2025-04-03</v>
+        <v>2025-04-11</v>
       </c>
     </row>
     <row r="42" spans="1:1" customFormat="false">
       <c r="A42" s="0" t="str">
-        <v>2025-04-04</v>
+        <v>2025-04-12</v>
       </c>
     </row>
     <row r="43" spans="1:1" customFormat="false">
       <c r="A43" s="0" t="str">
-        <v>2025-04-05</v>
+        <v>2025-04-13</v>
       </c>
     </row>
     <row r="44" spans="1:1" customFormat="false">
       <c r="A44" s="0" t="str">
-        <v>2025-04-06</v>
+        <v>2025-04-14</v>
       </c>
     </row>
     <row r="45" spans="1:1" customFormat="false">
       <c r="A45" s="0" t="str">
-        <v>2025-04-07</v>
+        <v>2025-04-15</v>
       </c>
     </row>
     <row r="46" spans="1:1" customFormat="false">
       <c r="A46" s="0" t="str">
-        <v>2025-04-08</v>
+        <v>2025-04-16</v>
       </c>
     </row>
     <row r="47" spans="1:1" customFormat="false">
       <c r="A47" s="0" t="str">
-        <v>2025-04-09</v>
+        <v>2025-04-17</v>
       </c>
     </row>
     <row r="48" spans="1:1" customFormat="false">
       <c r="A48" s="0" t="str">
-        <v>2025-04-10</v>
+        <v>2025-04-18</v>
       </c>
     </row>
     <row r="49" spans="1:1" customFormat="false">
       <c r="A49" s="0" t="str">
-        <v>2025-04-11</v>
+        <v>2025-04-19</v>
       </c>
     </row>
     <row r="50" spans="1:1" customFormat="false">
       <c r="A50" s="0" t="str">
-        <v>2025-04-12</v>
+        <v>2025-04-20</v>
       </c>
     </row>
     <row r="51" spans="1:1" customFormat="false">
       <c r="A51" s="0" t="str">
-        <v>2025-04-13</v>
+        <v>2025-04-21</v>
       </c>
     </row>
     <row r="52" spans="1:1" customFormat="false">
       <c r="A52" s="0" t="str">
-        <v>2025-04-14</v>
+        <v>2025-04-22</v>
       </c>
     </row>
     <row r="53" spans="1:1" customFormat="false">
       <c r="A53" s="0" t="str">
-        <v>2025-04-15</v>
+        <v>2025-04-23</v>
       </c>
     </row>
     <row r="54" spans="1:1" customFormat="false">
       <c r="A54" s="0" t="str">
-        <v>2025-04-16</v>
+        <v>2025-04-24</v>
       </c>
     </row>
     <row r="55" spans="1:1" customFormat="false">
       <c r="A55" s="0" t="str">
-        <v>2025-04-17</v>
+        <v>2025-04-25</v>
       </c>
     </row>
     <row r="56" spans="1:1" customFormat="false">
       <c r="A56" s="0" t="str">
-        <v>2025-04-18</v>
+        <v>2025-04-26</v>
       </c>
     </row>
     <row r="57" spans="1:1" customFormat="false">
       <c r="A57" s="0" t="str">
-        <v>2025-04-19</v>
+        <v>2025-04-27</v>
       </c>
     </row>
     <row r="58" spans="1:1" customFormat="false">
       <c r="A58" s="0" t="str">
-        <v>2025-04-20</v>
+        <v>2025-04-28</v>
       </c>
     </row>
     <row r="59" spans="1:1" customFormat="false">
       <c r="A59" s="0" t="str">
-        <v>2025-04-21</v>
+        <v>2025-04-29</v>
       </c>
     </row>
     <row r="60" spans="1:1" customFormat="false">
       <c r="A60" s="0" t="str">
-        <v>2025-04-22</v>
+        <v>2025-04-30</v>
       </c>
     </row>
     <row r="61" spans="1:1" customFormat="false">
       <c r="A61" s="0" t="str">
-        <v>2025-04-23</v>
+        <v>2025-05-01</v>
       </c>
     </row>
     <row r="62" spans="1:1" customFormat="false">
       <c r="A62" s="0" t="str">
-        <v>2025-04-24</v>
+        <v>2025-05-02</v>
       </c>
     </row>
     <row r="63" spans="1:1" customFormat="false">
       <c r="A63" s="0" t="str">
-        <v>2025-04-25</v>
+        <v>2025-05-03</v>
       </c>
     </row>
     <row r="64" spans="1:1" customFormat="false">
       <c r="A64" s="0" t="str">
-        <v>2025-04-26</v>
+        <v>2025-05-04</v>
       </c>
     </row>
     <row r="65" spans="1:1" customFormat="false">
       <c r="A65" s="0" t="str">
-        <v>2025-04-27</v>
+        <v>2025-05-05</v>
       </c>
     </row>
     <row r="66" spans="1:1" customFormat="false">
       <c r="A66" s="0" t="str">
-        <v>2025-04-28</v>
+        <v>2025-05-06</v>
       </c>
     </row>
     <row r="67" spans="1:1" customFormat="false">
       <c r="A67" s="0" t="str">
-        <v>2025-04-29</v>
+        <v>2025-05-07</v>
       </c>
     </row>
     <row r="68" spans="1:1" customFormat="false">
       <c r="A68" s="0" t="str">
-        <v>2025-04-30</v>
+        <v>2025-05-08</v>
       </c>
     </row>
     <row r="69" spans="1:1" customFormat="false">
       <c r="A69" s="0" t="str">
-        <v>2025-05-01</v>
+        <v>2025-05-09</v>
       </c>
     </row>
     <row r="70" spans="1:1" customFormat="false">
       <c r="A70" s="0" t="str">
-        <v>2025-05-02</v>
+        <v>2025-05-10</v>
       </c>
     </row>
     <row r="71" spans="1:1" customFormat="false">
       <c r="A71" s="0" t="str">
-        <v>2025-05-03</v>
+        <v>2025-05-11</v>
       </c>
     </row>
     <row r="72" spans="1:1" customFormat="false">
       <c r="A72" s="0" t="str">
-        <v>2025-05-04</v>
+        <v>2025-05-12</v>
       </c>
     </row>
     <row r="73" spans="1:1" customFormat="false">
       <c r="A73" s="0" t="str">
-        <v>2025-05-05</v>
+        <v>2025-05-13</v>
       </c>
     </row>
     <row r="74" spans="1:1" customFormat="false">
       <c r="A74" s="0" t="str">
-        <v>2025-05-06</v>
+        <v>2025-05-14</v>
       </c>
     </row>
     <row r="75" spans="1:1" customFormat="false">
       <c r="A75" s="0" t="str">
-        <v>2025-05-07</v>
+        <v>2025-05-15</v>
       </c>
     </row>
     <row r="76" spans="1:1" customFormat="false">
       <c r="A76" s="0" t="str">
-        <v>2025-05-08</v>
+        <v>2025-05-16</v>
       </c>
     </row>
     <row r="77" spans="1:1" customFormat="false">
       <c r="A77" s="0" t="str">
-        <v>2025-05-09</v>
+        <v>2025-05-17</v>
       </c>
     </row>
     <row r="78" spans="1:1" customFormat="false">
       <c r="A78" s="0" t="str">
-        <v>2025-05-10</v>
+        <v>2025-05-18</v>
       </c>
     </row>
     <row r="79" spans="1:1" customFormat="false">
       <c r="A79" s="0" t="str">
-        <v>2025-05-11</v>
+        <v>2025-05-19</v>
       </c>
     </row>
     <row r="80" spans="1:1" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>2025-05-12</v>
+        <v>2025-05-20</v>
       </c>
     </row>
     <row r="81" spans="1:1" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>2025-05-13</v>
+        <v>2025-05-21</v>
       </c>
     </row>
     <row r="82" spans="1:1" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>2025-05-14</v>
+        <v>2025-05-22</v>
       </c>
     </row>
     <row r="83" spans="1:1" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>2025-05-15</v>
+        <v>2025-05-23</v>
       </c>
     </row>
     <row r="84" spans="1:1" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>2025-05-16</v>
+        <v>2025-05-24</v>
       </c>
     </row>
     <row r="85" spans="1:1" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>2025-05-17</v>
+        <v>2025-05-25</v>
       </c>
     </row>
     <row r="86" spans="1:1" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>2025-05-18</v>
+        <v>2025-05-26</v>
       </c>
     </row>
     <row r="87" spans="1:1" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>2025-05-19</v>
+        <v>2025-05-27</v>
       </c>
     </row>
     <row r="88" spans="1:1" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>2025-05-20</v>
+        <v>2025-05-28</v>
       </c>
     </row>
     <row r="89" spans="1:1" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>2025-05-21</v>
+        <v>2025-05-29</v>
       </c>
     </row>
     <row r="90" spans="1:1" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>2025-05-22</v>
+        <v>2025-05-30</v>
       </c>
     </row>
     <row r="91" spans="1:1" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>2025-05-23</v>
+        <v>2025-05-31</v>
       </c>
     </row>
     <row r="92" spans="1:1" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>2025-05-24</v>
+        <v>2025-06-01</v>
       </c>
     </row>
     <row r="93" spans="1:1" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>2025-05-25</v>
+        <v>2025-06-02</v>
       </c>
     </row>
     <row r="94" spans="1:1" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>2025-05-26</v>
+        <v>2025-06-03</v>
       </c>
     </row>
     <row r="95" spans="1:1" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>2025-05-27</v>
+        <v>2025-06-04</v>
       </c>
     </row>
     <row r="96" spans="1:1" customFormat="false">
       <c r="A96" s="0" t="str">
-        <v>2025-05-28</v>
+        <v>2025-06-05</v>
       </c>
     </row>
     <row r="97" spans="1:1" customFormat="false">
       <c r="A97" s="0" t="str">
-        <v>2025-05-29</v>
+        <v>2025-06-06</v>
       </c>
     </row>
     <row r="98" spans="1:1" customFormat="false">
       <c r="A98" s="0" t="str">
-        <v>2025-05-30</v>
+        <v>2025-06-07</v>
       </c>
     </row>
     <row r="99" spans="1:1" customFormat="false">
       <c r="A99" s="0" t="str">
-        <v>2025-05-31</v>
+        <v>2025-06-08</v>
       </c>
     </row>
     <row r="100" spans="1:1" customFormat="false">
       <c r="A100" s="0" t="str">
-        <v>2025-06-01</v>
+        <v>2025-06-09</v>
       </c>
     </row>
     <row r="101" spans="1:1" customFormat="false">
       <c r="A101" s="0" t="str">
-        <v>2025-06-02</v>
+        <v>2025-06-10</v>
       </c>
     </row>
     <row r="102" spans="1:1" customFormat="false">
       <c r="A102" s="0" t="str">
-        <v>2025-06-03</v>
+        <v>2025-06-11</v>
       </c>
     </row>
     <row r="103" spans="1:1" customFormat="false">
       <c r="A103" s="0" t="str">
-        <v>2025-06-04</v>
+        <v>2025-06-12</v>
       </c>
     </row>
     <row r="104" spans="1:1" customFormat="false">
       <c r="A104" s="0" t="str">
-        <v>2025-06-05</v>
+        <v>2025-06-13</v>
       </c>
     </row>
     <row r="105" spans="1:1" customFormat="false">
       <c r="A105" s="0" t="str">
-        <v>2025-06-06</v>
+        <v>2025-06-14</v>
       </c>
     </row>
     <row r="106" spans="1:1" customFormat="false">
       <c r="A106" s="0" t="str">
-        <v>2025-06-07</v>
+        <v>2025-06-15</v>
       </c>
     </row>
     <row r="107" spans="1:1" customFormat="false">
       <c r="A107" s="0" t="str">
-        <v>2025-06-08</v>
+        <v>2025-06-16</v>
       </c>
     </row>
     <row r="108" spans="1:1" customFormat="false">
       <c r="A108" s="0" t="str">
-        <v>2025-06-09</v>
+        <v>2025-06-17</v>
       </c>
     </row>
     <row r="109" spans="1:1" customFormat="false">
       <c r="A109" s="0" t="str">
-        <v>2025-06-10</v>
+        <v>2025-06-18</v>
       </c>
     </row>
     <row r="110" spans="1:1" customFormat="false">
       <c r="A110" s="0" t="str">
-        <v>2025-06-11</v>
+        <v>2025-06-19</v>
       </c>
     </row>
     <row r="111" spans="1:1" customFormat="false">
       <c r="A111" s="0" t="str">
-        <v>2025-06-12</v>
+        <v>2025-06-20</v>
       </c>
     </row>
     <row r="112" spans="1:1" customFormat="false">
       <c r="A112" s="0" t="str">
-        <v>2025-06-13</v>
+        <v>2025-06-21</v>
       </c>
     </row>
     <row r="113" spans="1:1" customFormat="false">
       <c r="A113" s="0" t="str">
-        <v>2025-06-14</v>
+        <v>2025-06-22</v>
       </c>
     </row>
     <row r="114" spans="1:1" customFormat="false">
       <c r="A114" s="0" t="str">
-        <v>2025-06-15</v>
+        <v>2025-06-23</v>
       </c>
     </row>
     <row r="115" spans="1:1" customFormat="false">
       <c r="A115" s="0" t="str">
-        <v>2025-06-16</v>
+        <v>2025-06-24</v>
       </c>
     </row>
     <row r="116" spans="1:1" customFormat="false">
       <c r="A116" s="0" t="str">
-        <v>2025-06-17</v>
+        <v>2025-06-25</v>
       </c>
     </row>
     <row r="117" spans="1:1" customFormat="false">
       <c r="A117" s="0" t="str">
-        <v>2025-06-18</v>
+        <v>2025-06-26</v>
       </c>
     </row>
     <row r="118" spans="1:1" customFormat="false">
       <c r="A118" s="0" t="str">
-        <v>2025-06-19</v>
+        <v>2025-06-27</v>
       </c>
     </row>
     <row r="119" spans="1:1" customFormat="false">
       <c r="A119" s="0" t="str">
-        <v>2025-06-20</v>
+        <v>2025-06-28</v>
       </c>
     </row>
     <row r="120" spans="1:1" customFormat="false">
       <c r="A120" s="0" t="str">
-        <v>2025-06-21</v>
+        <v>2025-06-29</v>
       </c>
     </row>
     <row r="121" spans="1:1" customFormat="false">
       <c r="A121" s="0" t="str">
-        <v>2025-06-22</v>
+        <v>2025-06-30</v>
       </c>
     </row>
     <row r="122" spans="1:1" customFormat="false">
       <c r="A122" s="0" t="str">
-        <v>2025-06-23</v>
+        <v>2025-07-01</v>
       </c>
     </row>
     <row r="123" spans="1:1" customFormat="false">
       <c r="A123" s="0" t="str">
-        <v>2025-06-24</v>
+        <v>2025-07-02</v>
       </c>
     </row>
     <row r="124" spans="1:1" customFormat="false">
       <c r="A124" s="0" t="str">
-        <v>2025-06-25</v>
+        <v>2025-07-03</v>
       </c>
     </row>
     <row r="125" spans="1:1" customFormat="false">
       <c r="A125" s="0" t="str">
-        <v>2025-06-26</v>
+        <v>2025-07-04</v>
       </c>
     </row>
     <row r="126" spans="1:1" customFormat="false">
       <c r="A126" s="0" t="str">
-        <v>2025-06-27</v>
+        <v>2025-07-05</v>
       </c>
     </row>
     <row r="127" spans="1:1" customFormat="false">
       <c r="A127" s="0" t="str">
-        <v>2025-06-28</v>
+        <v>2025-07-06</v>
       </c>
     </row>
     <row r="128" spans="1:1" customFormat="false">
       <c r="A128" s="0" t="str">
-        <v>2025-06-29</v>
+        <v>2025-07-07</v>
       </c>
     </row>
     <row r="129" spans="1:1" customFormat="false">
       <c r="A129" s="0" t="str">
-        <v>2025-06-30</v>
+        <v>2025-07-08</v>
       </c>
     </row>
     <row r="130" spans="1:1" customFormat="false">
       <c r="A130" s="0" t="str">
-        <v>2025-07-01</v>
+        <v>2025-07-09</v>
       </c>
     </row>
     <row r="131" spans="1:1" customFormat="false">
       <c r="A131" s="0" t="str">
-        <v>2025-07-02</v>
+        <v>2025-07-10</v>
       </c>
     </row>
     <row r="132" spans="1:1" customFormat="false">
       <c r="A132" s="0" t="str">
-        <v>2025-07-03</v>
+        <v>2025-07-11</v>
       </c>
     </row>
     <row r="133" spans="1:1" customFormat="false">
       <c r="A133" s="0" t="str">
-        <v>2025-07-04</v>
+        <v>2025-07-12</v>
       </c>
     </row>
     <row r="134" spans="1:1" customFormat="false">
       <c r="A134" s="0" t="str">
-        <v>2025-07-05</v>
+        <v>2025-07-13</v>
       </c>
     </row>
     <row r="135" spans="1:1" customFormat="false">
       <c r="A135" s="0" t="str">
-        <v>2025-07-06</v>
+        <v>2025-07-14</v>
       </c>
     </row>
     <row r="136" spans="1:1" customFormat="false">
       <c r="A136" s="0" t="str">
-        <v>2025-07-07</v>
+        <v>2025-07-15</v>
       </c>
     </row>
     <row r="137" spans="1:1" customFormat="false">
       <c r="A137" s="0" t="str">
-        <v>2025-07-08</v>
+        <v>2025-07-16</v>
       </c>
     </row>
     <row r="138" spans="1:1" customFormat="false">
       <c r="A138" s="0" t="str">
-        <v>2025-07-09</v>
+        <v>2025-07-17</v>
       </c>
     </row>
     <row r="139" spans="1:1" customFormat="false">
       <c r="A139" s="0" t="str">
-        <v>2025-07-10</v>
+        <v>2025-07-18</v>
       </c>
     </row>
     <row r="140" spans="1:1" customFormat="false">
       <c r="A140" s="0" t="str">
-        <v>2025-07-11</v>
+        <v>2025-07-19</v>
       </c>
     </row>
     <row r="141" spans="1:1" customFormat="false">
       <c r="A141" s="0" t="str">
-        <v>2025-07-12</v>
+        <v>2025-07-20</v>
       </c>
     </row>
     <row r="142" spans="1:1" customFormat="false">
       <c r="A142" s="0" t="str">
-        <v>2025-07-13</v>
+        <v>2025-07-21</v>
       </c>
     </row>
     <row r="143" spans="1:1" customFormat="false">
       <c r="A143" s="0" t="str">
-        <v>2025-07-14</v>
+        <v>2025-07-22</v>
       </c>
     </row>
     <row r="144" spans="1:1" customFormat="false">
       <c r="A144" s="0" t="str">
-        <v>2025-07-15</v>
+        <v>2025-07-23</v>
       </c>
     </row>
     <row r="145" spans="1:1" customFormat="false">
       <c r="A145" s="0" t="str">
-        <v>2025-07-16</v>
+        <v>2025-07-24</v>
       </c>
     </row>
     <row r="146" spans="1:1" customFormat="false">
       <c r="A146" s="0" t="str">
-        <v>2025-07-17</v>
+        <v>2025-07-25</v>
       </c>
     </row>
     <row r="147" spans="1:1" customFormat="false">
       <c r="A147" s="0" t="str">
-        <v>2025-07-18</v>
+        <v>2025-07-26</v>
       </c>
     </row>
     <row r="148" spans="1:1" customFormat="false">
       <c r="A148" s="0" t="str">
-        <v>2025-07-19</v>
+        <v>2025-07-27</v>
       </c>
     </row>
     <row r="149" spans="1:1" customFormat="false">
       <c r="A149" s="0" t="str">
-        <v>2025-07-20</v>
+        <v>2025-07-28</v>
       </c>
     </row>
     <row r="150" spans="1:1" customFormat="false">
       <c r="A150" s="0" t="str">
-        <v>2025-07-21</v>
+        <v>2025-07-29</v>
       </c>
     </row>
     <row r="151" spans="1:1" customFormat="false">
       <c r="A151" s="0" t="str">
-        <v>2025-07-22</v>
+        <v>2025-07-30</v>
       </c>
     </row>
     <row r="152" spans="1:1" customFormat="false">
       <c r="A152" s="0" t="str">
-        <v>2025-07-23</v>
+        <v>2025-07-31</v>
       </c>
     </row>
     <row r="153" spans="1:1" customFormat="false">
       <c r="A153" s="0" t="str">
-        <v>2025-07-24</v>
+        <v>2025-08-01</v>
       </c>
     </row>
     <row r="154" spans="1:1" customFormat="false">
       <c r="A154" s="0" t="str">
-        <v>2025-07-25</v>
+        <v>2025-08-02</v>
       </c>
     </row>
     <row r="155" spans="1:1" customFormat="false">
       <c r="A155" s="0" t="str">
-        <v>2025-07-26</v>
+        <v>2025-08-03</v>
       </c>
     </row>
     <row r="156" spans="1:1" customFormat="false">
       <c r="A156" s="0" t="str">
-        <v>2025-07-27</v>
+        <v>2025-08-04</v>
       </c>
     </row>
     <row r="157" spans="1:1" customFormat="false">
       <c r="A157" s="0" t="str">
-        <v>2025-07-28</v>
+        <v>2025-08-05</v>
       </c>
     </row>
     <row r="158" spans="1:1" customFormat="false">
       <c r="A158" s="0" t="str">
-        <v>2025-07-29</v>
+        <v>2025-08-06</v>
       </c>
     </row>
     <row r="159" spans="1:1" customFormat="false">
       <c r="A159" s="0" t="str">
-        <v>2025-07-30</v>
+        <v>2025-08-07</v>
       </c>
     </row>
     <row r="160" spans="1:1" customFormat="false">
       <c r="A160" s="0" t="str">
-        <v>2025-07-31</v>
+        <v>2025-08-08</v>
       </c>
     </row>
     <row r="161" spans="1:1" customFormat="false">
       <c r="A161" s="0" t="str">
-        <v>2025-08-01</v>
+        <v>2025-08-09</v>
       </c>
     </row>
     <row r="162" spans="1:1" customFormat="false">
       <c r="A162" s="0" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-10</v>
       </c>
     </row>
     <row r="163" spans="1:1" customFormat="false">
       <c r="A163" s="0" t="str">
-        <v>2025-08-03</v>
+        <v>2025-08-11</v>
       </c>
     </row>
     <row r="164" spans="1:1" customFormat="false">
       <c r="A164" s="0" t="str">
-        <v>2025-08-04</v>
+        <v>2025-08-12</v>
       </c>
     </row>
     <row r="165" spans="1:1" customFormat="false">
       <c r="A165" s="0" t="str">
-        <v>2025-08-05</v>
+        <v>2025-08-13</v>
       </c>
     </row>
     <row r="166" spans="1:1" customFormat="false">
       <c r="A166" s="0" t="str">
-        <v>2025-08-06</v>
+        <v>2025-08-14</v>
       </c>
     </row>
     <row r="167" spans="1:1" customFormat="false">
       <c r="A167" s="0" t="str">
-        <v>2025-08-07</v>
+        <v>2025-08-15</v>
       </c>
     </row>
     <row r="168" spans="1:1" customFormat="false">
       <c r="A168" s="0" t="str">
-        <v>2025-08-08</v>
+        <v>2025-08-16</v>
       </c>
     </row>
     <row r="169" spans="1:1" customFormat="false">
       <c r="A169" s="0" t="str">
-        <v>2025-08-09</v>
+        <v>2025-08-17</v>
       </c>
     </row>
     <row r="170" spans="1:1" customFormat="false">
       <c r="A170" s="0" t="str">
-        <v>2025-08-10</v>
+        <v>2025-08-18</v>
       </c>
     </row>
     <row r="171" spans="1:1" customFormat="false">
       <c r="A171" s="0" t="str">
-        <v>2025-08-11</v>
+        <v>2025-08-19</v>
       </c>
     </row>
     <row r="172" spans="1:1" customFormat="false">
       <c r="A172" s="0" t="str">
-        <v>2025-08-12</v>
+        <v>2025-08-20</v>
       </c>
     </row>
     <row r="173" spans="1:1" customFormat="false">
       <c r="A173" s="0" t="str">
-        <v>2025-08-13</v>
+        <v>2025-08-21</v>
       </c>
     </row>
     <row r="174" spans="1:1" customFormat="false">
       <c r="A174" s="0" t="str">
-        <v>2025-08-14</v>
+        <v>2025-08-22</v>
       </c>
     </row>
     <row r="175" spans="1:1" customFormat="false">
       <c r="A175" s="0" t="str">
-        <v>2025-08-15</v>
+        <v>2025-08-23</v>
       </c>
     </row>
     <row r="176" spans="1:1" customFormat="false">
       <c r="A176" s="0" t="str">
-        <v>2025-08-16</v>
+        <v>2025-08-24</v>
       </c>
     </row>
     <row r="177" spans="1:1" customFormat="false">
       <c r="A177" s="0" t="str">
-        <v>2025-08-17</v>
+        <v>2025-08-25</v>
       </c>
     </row>
     <row r="178" spans="1:1" customFormat="false">
       <c r="A178" s="0" t="str">
-        <v>2025-08-18</v>
+        <v>2025-08-26</v>
       </c>
     </row>
     <row r="179" spans="1:1" customFormat="false">
       <c r="A179" s="0" t="str">
-        <v>2025-08-19</v>
+        <v>2025-08-27</v>
       </c>
     </row>
     <row r="180" spans="1:1" customFormat="false">
       <c r="A180" s="0" t="str">
-        <v>2025-08-20</v>
+        <v>2025-08-28</v>
       </c>
     </row>
     <row r="181" spans="1:1" customFormat="false">
       <c r="A181" s="0" t="str">
-        <v>2025-08-21</v>
+        <v>2025-08-29</v>
       </c>
     </row>
     <row r="182" spans="1:1" customFormat="false">
       <c r="A182" s="0" t="str">
-        <v>2025-08-22</v>
+        <v>2025-08-30</v>
       </c>
     </row>
     <row r="183" spans="1:1" customFormat="false">
       <c r="A183" s="0" t="str">
-        <v>2025-08-23</v>
+        <v>2025-08-31</v>
       </c>
     </row>
     <row r="184" spans="1:1" customFormat="false">
       <c r="A184" s="0" t="str">
-        <v>2025-08-24</v>
+        <v>2025-09-01</v>
       </c>
     </row>
     <row r="185" spans="1:1" customFormat="false">
       <c r="A185" s="0" t="str">
-        <v>2025-08-25</v>
+        <v>2025-09-02</v>
       </c>
     </row>
     <row r="186" spans="1:1" customFormat="false">
       <c r="A186" s="0" t="str">
-        <v>2025-08-26</v>
+        <v>2025-09-03</v>
       </c>
     </row>
     <row r="187" spans="1:1" customFormat="false">
       <c r="A187" s="0" t="str">
-        <v>2025-08-27</v>
+        <v>2025-09-04</v>
       </c>
     </row>
     <row r="188" spans="1:1" customFormat="false">
       <c r="A188" s="0" t="str">
-        <v>2025-08-28</v>
+        <v>2025-09-05</v>
       </c>
     </row>
     <row r="189" spans="1:1" customFormat="false">
       <c r="A189" s="0" t="str">
-        <v>2025-08-29</v>
+        <v>2025-09-06</v>
       </c>
     </row>
     <row r="190" spans="1:1" customFormat="false">
       <c r="A190" s="0" t="str">
-        <v>2025-08-30</v>
+        <v>2025-09-07</v>
       </c>
     </row>
     <row r="191" spans="1:1" customFormat="false">
       <c r="A191" s="0" t="str">
-        <v>2025-08-31</v>
+        <v>2025-09-08</v>
       </c>
     </row>
     <row r="192" spans="1:1" customFormat="false">
       <c r="A192" s="0" t="str">
-        <v>2025-09-01</v>
+        <v>2025-09-09</v>
       </c>
     </row>
     <row r="193" spans="1:1" customFormat="false">
       <c r="A193" s="0" t="str">
-        <v>2025-09-02</v>
+        <v>2025-09-10</v>
       </c>
     </row>
     <row r="194" spans="1:1" customFormat="false">
       <c r="A194" s="0" t="str">
-        <v>2025-09-03</v>
+        <v>2025-09-11</v>
       </c>
     </row>
     <row r="195" spans="1:1" customFormat="false">
       <c r="A195" s="0" t="str">
-        <v>2025-09-04</v>
+        <v>2025-09-12</v>
       </c>
     </row>
     <row r="196" spans="1:1" customFormat="false">
       <c r="A196" s="0" t="str">
-        <v>2025-09-05</v>
+        <v>2025-09-13</v>
       </c>
     </row>
     <row r="197" spans="1:1" customFormat="false">
       <c r="A197" s="0" t="str">
-        <v>2025-09-06</v>
+        <v>2025-09-14</v>
       </c>
     </row>
     <row r="198" spans="1:1" customFormat="false">
       <c r="A198" s="0" t="str">
-        <v>2025-09-07</v>
+        <v>2025-09-15</v>
       </c>
     </row>
     <row r="199" spans="1:1" customFormat="false">
       <c r="A199" s="0" t="str">
-        <v>2025-09-08</v>
+        <v>2025-09-16</v>
       </c>
     </row>
     <row r="200" spans="1:1" customFormat="false">
       <c r="A200" s="0" t="str">
-        <v>2025-09-09</v>
+        <v>2025-09-17</v>
       </c>
     </row>
     <row r="201" spans="1:1" customFormat="false">
       <c r="A201" s="0" t="str">
-        <v>2025-09-10</v>
+        <v>2025-09-18</v>
       </c>
     </row>
     <row r="202" spans="1:1" customFormat="false">
       <c r="A202" s="0" t="str">
-        <v>2025-09-11</v>
+        <v>2025-09-19</v>
       </c>
     </row>
     <row r="203" spans="1:1" customFormat="false">
       <c r="A203" s="0" t="str">
-        <v>2025-09-12</v>
+        <v>2025-09-20</v>
       </c>
     </row>
     <row r="204" spans="1:1" customFormat="false">
       <c r="A204" s="0" t="str">
-        <v>2025-09-13</v>
+        <v>2025-09-21</v>
       </c>
     </row>
     <row r="205" spans="1:1" customFormat="false">
       <c r="A205" s="0" t="str">
-        <v>2025-09-14</v>
+        <v>2025-09-22</v>
       </c>
     </row>
     <row r="206" spans="1:1" customFormat="false">
       <c r="A206" s="0" t="str">
-        <v>2025-09-15</v>
+        <v>2025-09-23</v>
       </c>
     </row>
     <row r="207" spans="1:1" customFormat="false">
       <c r="A207" s="0" t="str">
-        <v>2025-09-16</v>
+        <v>2025-09-24</v>
       </c>
     </row>
     <row r="208" spans="1:1" customFormat="false">
       <c r="A208" s="0" t="str">
-        <v>2025-09-17</v>
+        <v>2025-09-25</v>
       </c>
     </row>
     <row r="209" spans="1:1" customFormat="false">
       <c r="A209" s="0" t="str">
-        <v>2025-09-18</v>
+        <v>2025-09-26</v>
       </c>
     </row>
     <row r="210" spans="1:1" customFormat="false">
       <c r="A210" s="0" t="str">
-        <v>2025-09-19</v>
+        <v>2025-09-27</v>
       </c>
     </row>
     <row r="211" spans="1:1" customFormat="false">
       <c r="A211" s="0" t="str">
-        <v>2025-09-20</v>
+        <v>2025-09-28</v>
       </c>
     </row>
     <row r="212" spans="1:1" customFormat="false">
       <c r="A212" s="0" t="str">
-        <v>2025-09-21</v>
+        <v>2025-09-29</v>
       </c>
     </row>
     <row r="213" spans="1:1" customFormat="false">
       <c r="A213" s="0" t="str">
-        <v>2025-09-22</v>
+        <v>2025-09-30</v>
       </c>
     </row>
     <row r="214" spans="1:1" customFormat="false">
       <c r="A214" s="0" t="str">
-        <v>2025-09-23</v>
+        <v>2025-10-01</v>
       </c>
     </row>
     <row r="215" spans="1:1" customFormat="false">
       <c r="A215" s="0" t="str">
-        <v>2025-09-24</v>
+        <v>2025-10-02</v>
       </c>
     </row>
     <row r="216" spans="1:1" customFormat="false">
       <c r="A216" s="0" t="str">
-        <v>2025-09-25</v>
+        <v>2025-10-03</v>
       </c>
     </row>
     <row r="217" spans="1:1" customFormat="false">
       <c r="A217" s="0" t="str">
-        <v>2025-09-26</v>
+        <v>2025-10-04</v>
       </c>
     </row>
     <row r="218" spans="1:1" customFormat="false">
       <c r="A218" s="0" t="str">
-        <v>2025-09-27</v>
+        <v>2025-10-05</v>
       </c>
     </row>
     <row r="219" spans="1:1" customFormat="false">
       <c r="A219" s="0" t="str">
-        <v>2025-09-28</v>
+        <v>2025-10-06</v>
       </c>
     </row>
     <row r="220" spans="1:1" customFormat="false">
       <c r="A220" s="0" t="str">
-        <v>2025-09-29</v>
+        <v>2025-10-07</v>
       </c>
     </row>
     <row r="221" spans="1:1" customFormat="false">
       <c r="A221" s="0" t="str">
-        <v>2025-09-30</v>
+        <v>2025-10-08</v>
       </c>
     </row>
     <row r="222" spans="1:1" customFormat="false">
       <c r="A222" s="0" t="str">
-        <v>2025-10-01</v>
+        <v>2025-10-09</v>
       </c>
     </row>
     <row r="223" spans="1:1" customFormat="false">
       <c r="A223" s="0" t="str">
-        <v>2025-10-02</v>
+        <v>2025-10-10</v>
       </c>
     </row>
     <row r="224" spans="1:1" customFormat="false">
       <c r="A224" s="0" t="str">
-        <v>2025-10-03</v>
+        <v>2025-10-11</v>
       </c>
     </row>
     <row r="225" spans="1:1" customFormat="false">
       <c r="A225" s="0" t="str">
-        <v>2025-10-04</v>
+        <v>2025-10-12</v>
       </c>
     </row>
     <row r="226" spans="1:1" customFormat="false">
       <c r="A226" s="0" t="str">
-        <v>2025-10-05</v>
+        <v>2025-10-13</v>
       </c>
     </row>
     <row r="227" spans="1:1" customFormat="false">
       <c r="A227" s="0" t="str">
-        <v>2025-10-06</v>
+        <v>2025-10-14</v>
       </c>
     </row>
     <row r="228" spans="1:1" customFormat="false">
       <c r="A228" s="0" t="str">
-        <v>2025-10-07</v>
+        <v>2025-10-15</v>
       </c>
     </row>
     <row r="229" spans="1:1" customFormat="false">
       <c r="A229" s="0" t="str">
-        <v>2025-10-08</v>
+        <v>2025-10-16</v>
       </c>
     </row>
     <row r="230" spans="1:1" customFormat="false">
       <c r="A230" s="0" t="str">
-        <v>2025-10-09</v>
+        <v>2025-10-17</v>
       </c>
     </row>
     <row r="231" spans="1:1" customFormat="false">
       <c r="A231" s="0" t="str">
-        <v>2025-10-10</v>
+        <v>2025-10-18</v>
       </c>
     </row>
     <row r="232" spans="1:1" customFormat="false">
       <c r="A232" s="0" t="str">
-        <v>2025-10-11</v>
+        <v>2025-10-19</v>
       </c>
     </row>
     <row r="233" spans="1:1" customFormat="false">
       <c r="A233" s="0" t="str">
-        <v>2025-10-12</v>
+        <v>2025-10-20</v>
       </c>
     </row>
     <row r="234" spans="1:1" customFormat="false">
       <c r="A234" s="0" t="str">
-        <v>2025-10-13</v>
+        <v>2025-10-21</v>
       </c>
     </row>
     <row r="235" spans="1:1" customFormat="false">
       <c r="A235" s="0" t="str">
-        <v>2025-10-14</v>
+        <v>2025-10-22</v>
       </c>
     </row>
     <row r="236" spans="1:1" customFormat="false">
       <c r="A236" s="0" t="str">
-        <v>2025-10-15</v>
+        <v>2025-10-23</v>
       </c>
     </row>
     <row r="237" spans="1:1" customFormat="false">
       <c r="A237" s="0" t="str">
-        <v>2025-10-16</v>
+        <v>2025-10-24</v>
       </c>
     </row>
     <row r="238" spans="1:1" customFormat="false">
       <c r="A238" s="0" t="str">
-        <v>2025-10-17</v>
+        <v>2025-10-25</v>
       </c>
     </row>
     <row r="239" spans="1:1" customFormat="false">
       <c r="A239" s="0" t="str">
-        <v>2025-10-18</v>
+        <v>2025-10-26</v>
       </c>
     </row>
     <row r="240" spans="1:1" customFormat="false">
       <c r="A240" s="0" t="str">
-        <v>2025-10-19</v>
+        <v>2025-10-27</v>
       </c>
     </row>
     <row r="241" spans="1:1" customFormat="false">
       <c r="A241" s="0" t="str">
-        <v>2025-10-20</v>
+        <v>2025-10-28</v>
       </c>
     </row>
     <row r="242" spans="1:1" customFormat="false">
       <c r="A242" s="0" t="str">
-        <v>2025-10-21</v>
+        <v>2025-10-29</v>
       </c>
     </row>
     <row r="243" spans="1:1" customFormat="false">
       <c r="A243" s="0" t="str">
-        <v>2025-10-22</v>
+        <v>2025-10-30</v>
       </c>
     </row>
     <row r="244" spans="1:1" customFormat="false">
       <c r="A244" s="0" t="str">
-        <v>2025-10-23</v>
+        <v>2025-10-31</v>
       </c>
     </row>
     <row r="245" spans="1:1" customFormat="false">
       <c r="A245" s="0" t="str">
-        <v>2025-10-24</v>
+        <v>2025-11-01</v>
       </c>
     </row>
     <row r="246" spans="1:1" customFormat="false">
       <c r="A246" s="0" t="str">
-        <v>2025-10-25</v>
+        <v>2025-11-02</v>
       </c>
     </row>
     <row r="247" spans="1:1" customFormat="false">
       <c r="A247" s="0" t="str">
-        <v>2025-10-26</v>
+        <v>2025-11-03</v>
       </c>
     </row>
     <row r="248" spans="1:1" customFormat="false">
       <c r="A248" s="0" t="str">
-        <v>2025-10-27</v>
+        <v>2025-11-04</v>
       </c>
     </row>
     <row r="249" spans="1:1" customFormat="false">
       <c r="A249" s="0" t="str">
-        <v>2025-10-28</v>
+        <v>2025-11-05</v>
       </c>
     </row>
     <row r="250" spans="1:1" customFormat="false">
       <c r="A250" s="0" t="str">
-        <v>2025-10-29</v>
+        <v>2025-11-06</v>
       </c>
     </row>
     <row r="251" spans="1:1" customFormat="false">
       <c r="A251" s="0" t="str">
-        <v>2025-10-30</v>
+        <v>2025-11-07</v>
       </c>
     </row>
     <row r="252" spans="1:1" customFormat="false">
       <c r="A252" s="0" t="str">
-        <v>2025-10-31</v>
+        <v>2025-11-08</v>
       </c>
     </row>
     <row r="253" spans="1:1" customFormat="false">
       <c r="A253" s="0" t="str">
-        <v>2025-11-01</v>
+        <v>2025-11-09</v>
       </c>
     </row>
     <row r="254" spans="1:1" customFormat="false">
       <c r="A254" s="0" t="str">
-        <v>2025-11-02</v>
+        <v>2025-11-10</v>
       </c>
     </row>
     <row r="255" spans="1:1" customFormat="false">
       <c r="A255" s="0" t="str">
-        <v>2025-11-03</v>
+        <v>2025-11-11</v>
       </c>
     </row>
     <row r="256" spans="1:1" customFormat="false">
       <c r="A256" s="0" t="str">
-        <v>2025-11-04</v>
+        <v>2025-11-12</v>
       </c>
     </row>
     <row r="257" spans="1:1" customFormat="false">
       <c r="A257" s="0" t="str">
-        <v>2025-11-05</v>
+        <v>2025-11-13</v>
       </c>
     </row>
     <row r="258" spans="1:1" customFormat="false">
       <c r="A258" s="0" t="str">
-        <v>2025-11-06</v>
+        <v>2025-11-14</v>
       </c>
     </row>
     <row r="259" spans="1:1" customFormat="false">
       <c r="A259" s="0" t="str">
-        <v>2025-11-07</v>
+        <v>2025-11-15</v>
       </c>
     </row>
     <row r="260" spans="1:1" customFormat="false">
       <c r="A260" s="0" t="str">
-        <v>2025-11-08</v>
+        <v>2025-11-16</v>
       </c>
     </row>
     <row r="261" spans="1:1" customFormat="false">
       <c r="A261" s="0" t="str">
-        <v>2025-11-09</v>
+        <v>2025-11-17</v>
       </c>
     </row>
     <row r="262" spans="1:1" customFormat="false">
       <c r="A262" s="0" t="str">
-        <v>2025-11-10</v>
+        <v>2025-11-18</v>
       </c>
     </row>
     <row r="263" spans="1:1" customFormat="false">
       <c r="A263" s="0" t="str">
-        <v>2025-11-11</v>
+        <v>2025-11-19</v>
       </c>
     </row>
     <row r="264" spans="1:1" customFormat="false">
       <c r="A264" s="0" t="str">
-        <v>2025-11-12</v>
+        <v>2025-11-20</v>
       </c>
     </row>
     <row r="265" spans="1:1" customFormat="false">
       <c r="A265" s="0" t="str">
-        <v>2025-11-13</v>
+        <v>2025-11-21</v>
       </c>
     </row>
     <row r="266" spans="1:1" customFormat="false">
       <c r="A266" s="0" t="str">
-        <v>2025-11-14</v>
+        <v>2025-11-22</v>
       </c>
     </row>
     <row r="267" spans="1:1" customFormat="false">
       <c r="A267" s="0" t="str">
-        <v>2025-11-15</v>
+        <v>2025-11-23</v>
       </c>
     </row>
     <row r="268" spans="1:1" customFormat="false">
       <c r="A268" s="0" t="str">
-        <v>2025-11-16</v>
+        <v>2025-11-24</v>
       </c>
     </row>
     <row r="269" spans="1:1" customFormat="false">
       <c r="A269" s="0" t="str">
-        <v>2025-11-17</v>
+        <v>2025-11-25</v>
       </c>
     </row>
     <row r="270" spans="1:1" customFormat="false">
       <c r="A270" s="0" t="str">
-        <v>2025-11-18</v>
+        <v>2025-11-26</v>
       </c>
     </row>
     <row r="271" spans="1:1" customFormat="false">
       <c r="A271" s="0" t="str">
-        <v>2025-11-19</v>
+        <v>2025-11-27</v>
       </c>
     </row>
     <row r="272" spans="1:1" customFormat="false">
       <c r="A272" s="0" t="str">
-        <v>2025-11-20</v>
+        <v>2025-11-28</v>
       </c>
     </row>
     <row r="273" spans="1:1" customFormat="false">
       <c r="A273" s="0" t="str">
-        <v>2025-11-21</v>
+        <v>2025-11-29</v>
       </c>
     </row>
     <row r="274" spans="1:1" customFormat="false">
       <c r="A274" s="0" t="str">
-        <v>2025-11-22</v>
+        <v>2025-11-30</v>
       </c>
     </row>
     <row r="275" spans="1:1" customFormat="false">
       <c r="A275" s="0" t="str">
-        <v>2025-11-23</v>
+        <v>2025-12-01</v>
       </c>
     </row>
     <row r="276" spans="1:1" customFormat="false">
       <c r="A276" s="0" t="str">
-        <v>2025-11-24</v>
+        <v>2025-12-02</v>
       </c>
     </row>
     <row r="277" spans="1:1" customFormat="false">
       <c r="A277" s="0" t="str">
-        <v>2025-11-25</v>
+        <v>2025-12-03</v>
       </c>
     </row>
     <row r="278" spans="1:1" customFormat="false">
       <c r="A278" s="0" t="str">
-        <v>2025-11-26</v>
+        <v>2025-12-04</v>
       </c>
     </row>
     <row r="279" spans="1:1" customFormat="false">
       <c r="A279" s="0" t="str">
-        <v>2025-11-27</v>
+        <v>2025-12-05</v>
       </c>
     </row>
     <row r="280" spans="1:1" customFormat="false">
       <c r="A280" s="0" t="str">
-        <v>2025-11-28</v>
+        <v>2025-12-06</v>
       </c>
     </row>
     <row r="281" spans="1:1" customFormat="false">
       <c r="A281" s="0" t="str">
-        <v>2025-11-29</v>
+        <v>2025-12-07</v>
       </c>
     </row>
     <row r="282" spans="1:1" customFormat="false">
       <c r="A282" s="0" t="str">
-        <v>2025-11-30</v>
+        <v>2025-12-08</v>
       </c>
     </row>
     <row r="283" spans="1:1" customFormat="false">
       <c r="A283" s="0" t="str">
-        <v>2025-12-01</v>
+        <v>2025-12-09</v>
       </c>
     </row>
     <row r="284" spans="1:1" customFormat="false">
       <c r="A284" s="0" t="str">
-        <v>2025-12-02</v>
+        <v>2025-12-10</v>
       </c>
     </row>
     <row r="285" spans="1:1" customFormat="false">
       <c r="A285" s="0" t="str">
-        <v>2025-12-03</v>
+        <v>2025-12-11</v>
       </c>
     </row>
     <row r="286" spans="1:1" customFormat="false">
       <c r="A286" s="0" t="str">
-        <v>2025-12-04</v>
+        <v>2025-12-12</v>
       </c>
     </row>
     <row r="287" spans="1:1" customFormat="false">
       <c r="A287" s="0" t="str">
-        <v>2025-12-05</v>
+        <v>2025-12-13</v>
       </c>
     </row>
     <row r="288" spans="1:1" customFormat="false">
       <c r="A288" s="0" t="str">
-        <v>2025-12-06</v>
+        <v>2025-12-14</v>
       </c>
     </row>
     <row r="289" spans="1:1" customFormat="false">
       <c r="A289" s="0" t="str">
-        <v>2025-12-07</v>
+        <v>2025-12-15</v>
       </c>
     </row>
     <row r="290" spans="1:1" customFormat="false">
       <c r="A290" s="0" t="str">
-        <v>2025-12-08</v>
+        <v>2025-12-16</v>
       </c>
     </row>
     <row r="291" spans="1:1" customFormat="false">
       <c r="A291" s="0" t="str">
-        <v>2025-12-09</v>
+        <v>2025-12-17</v>
       </c>
     </row>
     <row r="292" spans="1:1" customFormat="false">
       <c r="A292" s="0" t="str">
-        <v>2025-12-10</v>
+        <v>2025-12-18</v>
       </c>
     </row>
     <row r="293" spans="1:1" customFormat="false">
       <c r="A293" s="0" t="str">
-        <v>2025-12-11</v>
+        <v>2025-12-19</v>
       </c>
     </row>
     <row r="294" spans="1:1" customFormat="false">
       <c r="A294" s="0" t="str">
-        <v>2025-12-12</v>
+        <v>2025-12-20</v>
       </c>
     </row>
     <row r="295" spans="1:1" customFormat="false">
       <c r="A295" s="0" t="str">
-        <v>2025-12-13</v>
+        <v>2025-12-21</v>
       </c>
     </row>
     <row r="296" spans="1:1" customFormat="false">
       <c r="A296" s="0" t="str">
-        <v>2025-12-14</v>
+        <v>2025-12-22</v>
       </c>
     </row>
     <row r="297" spans="1:1" customFormat="false">
       <c r="A297" s="0" t="str">
-        <v>2025-12-15</v>
+        <v>2025-12-23</v>
       </c>
     </row>
     <row r="298" spans="1:1" customFormat="false">
       <c r="A298" s="0" t="str">
-        <v>2025-12-16</v>
+        <v>2025-12-24</v>
       </c>
     </row>
     <row r="299" spans="1:1" customFormat="false">
       <c r="A299" s="0" t="str">
-        <v>2025-12-17</v>
+        <v>2025-12-25</v>
       </c>
     </row>
     <row r="300" spans="1:1" customFormat="false">
       <c r="A300" s="0" t="str">
-        <v>2025-12-18</v>
+        <v>2025-12-26</v>
       </c>
     </row>
     <row r="301" spans="1:1" customFormat="false">
       <c r="A301" s="0" t="str">
-        <v>2025-12-19</v>
+        <v>2025-12-27</v>
       </c>
     </row>
     <row r="302" spans="1:1" customFormat="false">
       <c r="A302" s="0" t="str">
-        <v>2025-12-20</v>
+        <v>2025-12-28</v>
       </c>
     </row>
     <row r="303" spans="1:1" customFormat="false">
       <c r="A303" s="0" t="str">
-        <v>2025-12-21</v>
+        <v>2025-12-29</v>
       </c>
     </row>
     <row r="304" spans="1:1" customFormat="false">
       <c r="A304" s="0" t="str">
-        <v>2025-12-22</v>
+        <v>2025-12-30</v>
       </c>
     </row>
     <row r="305" spans="1:1" customFormat="false">
       <c r="A305" s="0" t="str">
-        <v>2025-12-23</v>
+        <v>2025-12-31</v>
       </c>
     </row>
     <row r="306" spans="1:1" customFormat="false">
       <c r="A306" s="0" t="str">
-        <v>2025-12-24</v>
+        <v>2026-01-01</v>
       </c>
     </row>
     <row r="307" spans="1:1" customFormat="false">
       <c r="A307" s="0" t="str">
-        <v>2025-12-25</v>
+        <v>2026-01-02</v>
       </c>
     </row>
     <row r="308" spans="1:1" customFormat="false">
       <c r="A308" s="0" t="str">
-        <v>2025-12-26</v>
+        <v>2026-01-03</v>
       </c>
     </row>
     <row r="309" spans="1:1" customFormat="false">
       <c r="A309" s="0" t="str">
-        <v>2025-12-27</v>
+        <v>2026-01-04</v>
       </c>
     </row>
     <row r="310" spans="1:1" customFormat="false">
       <c r="A310" s="0" t="str">
-        <v>2025-12-28</v>
+        <v>2026-01-05</v>
       </c>
     </row>
     <row r="311" spans="1:1" customFormat="false">
       <c r="A311" s="0" t="str">
-        <v>2025-12-29</v>
+        <v>2026-01-06</v>
       </c>
     </row>
     <row r="312" spans="1:1" customFormat="false">
       <c r="A312" s="0" t="str">
-        <v>2025-12-30</v>
+        <v>2026-01-07</v>
       </c>
     </row>
     <row r="313" spans="1:1" customFormat="false">
       <c r="A313" s="0" t="str">
-        <v>2025-12-31</v>
+        <v>2026-01-08</v>
       </c>
     </row>
     <row r="314" spans="1:1" customFormat="false">
       <c r="A314" s="0" t="str">
-        <v>2026-01-01</v>
+        <v>2026-01-09</v>
       </c>
     </row>
     <row r="315" spans="1:1" customFormat="false">
       <c r="A315" s="0" t="str">
-        <v>2026-01-02</v>
+        <v>2026-01-10</v>
       </c>
     </row>
     <row r="316" spans="1:1" customFormat="false">
       <c r="A316" s="0" t="str">
-        <v>2026-01-03</v>
+        <v>2026-01-11</v>
       </c>
     </row>
     <row r="317" spans="1:1" customFormat="false">
       <c r="A317" s="0" t="str">
-        <v>2026-01-04</v>
+        <v>2026-01-12</v>
       </c>
     </row>
     <row r="318" spans="1:1" customFormat="false">
       <c r="A318" s="0" t="str">
-        <v>2026-01-05</v>
+        <v>2026-01-13</v>
       </c>
     </row>
     <row r="319" spans="1:1" customFormat="false">
       <c r="A319" s="0" t="str">
-        <v>2026-01-06</v>
+        <v>2026-01-14</v>
       </c>
     </row>
     <row r="320" spans="1:1" customFormat="false">
       <c r="A320" s="0" t="str">
-        <v>2026-01-07</v>
+        <v>2026-01-15</v>
       </c>
     </row>
     <row r="321" spans="1:1" customFormat="false">
       <c r="A321" s="0" t="str">
-        <v>2026-01-08</v>
+        <v>2026-01-16</v>
       </c>
     </row>
     <row r="322" spans="1:1" customFormat="false">
       <c r="A322" s="0" t="str">
-        <v>2026-01-09</v>
+        <v>2026-01-17</v>
       </c>
     </row>
     <row r="323" spans="1:1" customFormat="false">
       <c r="A323" s="0" t="str">
-        <v>2026-01-10</v>
+        <v>2026-01-18</v>
       </c>
     </row>
     <row r="324" spans="1:1" customFormat="false">
       <c r="A324" s="0" t="str">
-        <v>2026-01-11</v>
+        <v>2026-01-19</v>
       </c>
     </row>
     <row r="325" spans="1:1" customFormat="false">
       <c r="A325" s="0" t="str">
-        <v>2026-01-12</v>
+        <v>2026-01-20</v>
       </c>
     </row>
     <row r="326" spans="1:1" customFormat="false">
       <c r="A326" s="0" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-21</v>
       </c>
     </row>
     <row r="327" spans="1:1" customFormat="false">
       <c r="A327" s="0" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-22</v>
       </c>
     </row>
     <row r="328" spans="1:1" customFormat="false">
       <c r="A328" s="0" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-23</v>
       </c>
     </row>
     <row r="329" spans="1:1" customFormat="false">
       <c r="A329" s="0" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-24</v>
       </c>
     </row>
     <row r="330" spans="1:1" customFormat="false">
       <c r="A330" s="0" t="str">
-        <v>2026-01-17</v>
+        <v>2026-01-25</v>
       </c>
     </row>
     <row r="331" spans="1:1" customFormat="false">
       <c r="A331" s="0" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-26</v>
       </c>
     </row>
     <row r="332" spans="1:1" customFormat="false">
       <c r="A332" s="0" t="str">
-        <v>2026-01-19</v>
+        <v>2026-01-27</v>
       </c>
     </row>
     <row r="333" spans="1:1" customFormat="false">
       <c r="A333" s="0" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-28</v>
       </c>
     </row>
     <row r="334" spans="1:1" customFormat="false">
       <c r="A334" s="0" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-29</v>
       </c>
     </row>
     <row r="335" spans="1:1" customFormat="false">
       <c r="A335" s="0" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-30</v>
       </c>
     </row>
     <row r="336" spans="1:1" customFormat="false">
       <c r="A336" s="0" t="str">
-        <v>2026-01-23</v>
+        <v>2026-01-31</v>
       </c>
     </row>
     <row r="337" spans="1:1" customFormat="false">
       <c r="A337" s="0" t="str">
-        <v>2026-01-24</v>
+        <v>2026-02-01</v>
       </c>
     </row>
     <row r="338" spans="1:1" customFormat="false">
       <c r="A338" s="0" t="str">
-        <v>2026-01-25</v>
+        <v>2026-02-02</v>
       </c>
     </row>
     <row r="339" spans="1:1" customFormat="false">
       <c r="A339" s="0" t="str">
-        <v>2026-01-26</v>
+        <v>2026-02-03</v>
       </c>
     </row>
     <row r="340" spans="1:1" customFormat="false">
       <c r="A340" s="0" t="str">
-        <v>2026-01-27</v>
+        <v>2026-02-04</v>
       </c>
     </row>
     <row r="341" spans="1:1" customFormat="false">
       <c r="A341" s="0" t="str">
-        <v>2026-01-28</v>
+        <v>2026-02-05</v>
       </c>
     </row>
     <row r="342" spans="1:1" customFormat="false">
       <c r="A342" s="0" t="str">
-        <v>2026-01-29</v>
+        <v>2026-02-06</v>
       </c>
     </row>
     <row r="343" spans="1:1" customFormat="false">
       <c r="A343" s="0" t="str">
-        <v>2026-01-30</v>
+        <v>2026-02-07</v>
       </c>
     </row>
     <row r="344" spans="1:1" customFormat="false">
       <c r="A344" s="0" t="str">
-        <v>2026-01-31</v>
+        <v>2026-02-08</v>
       </c>
     </row>
     <row r="345" spans="1:1" customFormat="false">
       <c r="A345" s="0" t="str">
-        <v>2026-02-01</v>
+        <v>2026-02-09</v>
       </c>
     </row>
     <row r="346" spans="1:1" customFormat="false">
       <c r="A346" s="0" t="str">
-        <v>2026-02-02</v>
+        <v>2026-02-10</v>
       </c>
     </row>
     <row r="347" spans="1:1" customFormat="false">
       <c r="A347" s="0" t="str">
-        <v>2026-02-03</v>
+        <v>2026-02-11</v>
       </c>
     </row>
     <row r="348" spans="1:1" customFormat="false">
       <c r="A348" s="0" t="str">
-        <v>2026-02-04</v>
+        <v>2026-02-12</v>
       </c>
     </row>
     <row r="349" spans="1:1" customFormat="false">
       <c r="A349" s="0" t="str">
-        <v>2026-02-05</v>
+        <v>2026-02-13</v>
       </c>
     </row>
     <row r="350" spans="1:1" customFormat="false">
       <c r="A350" s="0" t="str">
-        <v>2026-02-06</v>
+        <v>2026-02-14</v>
       </c>
     </row>
     <row r="351" spans="1:1" customFormat="false">
       <c r="A351" s="0" t="str">
-        <v>2026-02-07</v>
+        <v>2026-02-15</v>
       </c>
     </row>
     <row r="352" spans="1:1" customFormat="false">
       <c r="A352" s="0" t="str">
-        <v>2026-02-08</v>
+        <v>2026-02-16</v>
       </c>
     </row>
     <row r="353" spans="1:1" customFormat="false">
       <c r="A353" s="0" t="str">
-        <v>2026-02-09</v>
+        <v>2026-02-17</v>
       </c>
     </row>
     <row r="354" spans="1:1" customFormat="false">
       <c r="A354" s="0" t="str">
-        <v>2026-02-10</v>
+        <v>2026-02-18</v>
       </c>
     </row>
     <row r="355" spans="1:1" customFormat="false">
       <c r="A355" s="0" t="str">
-        <v>2026-02-11</v>
+        <v>2026-02-19</v>
       </c>
     </row>
     <row r="356" spans="1:1" customFormat="false">
       <c r="A356" s="0" t="str">
-        <v>2026-02-12</v>
+        <v>2026-02-20</v>
       </c>
     </row>
     <row r="357" spans="1:1" customFormat="false">
       <c r="A357" s="0" t="str">
-        <v>2026-02-13</v>
+        <v>2026-02-21</v>
       </c>
     </row>
     <row r="358" spans="1:1" customFormat="false">
       <c r="A358" s="0" t="str">
-        <v>2026-02-14</v>
+        <v>2026-02-22</v>
       </c>
     </row>
     <row r="359" spans="1:1" customFormat="false">
       <c r="A359" s="0" t="str">
-        <v>2026-02-15</v>
+        <v>2026-02-23</v>
       </c>
     </row>
     <row r="360" spans="1:1" customFormat="false">
       <c r="A360" s="0" t="str">
-        <v>2026-02-16</v>
+        <v>2026-02-24</v>
       </c>
     </row>
     <row r="361" spans="1:1" customFormat="false">
       <c r="A361" s="0" t="str">
-        <v>2026-02-17</v>
+        <v>2026-02-25</v>
       </c>
     </row>
     <row r="362" spans="1:1" customFormat="false">
       <c r="A362" s="0" t="str">
-        <v>2026-02-18</v>
+        <v>2026-02-26</v>
       </c>
     </row>
     <row r="363" spans="1:1" customFormat="false">
       <c r="A363" s="0" t="str">
-        <v>2026-02-19</v>
+        <v>2026-02-27</v>
       </c>
     </row>
     <row r="364" spans="1:1" customFormat="false">
       <c r="A364" s="0" t="str">
-        <v>2026-02-20</v>
+        <v>2026-02-28</v>
       </c>
     </row>
     <row r="365" spans="1:1" customFormat="false">
       <c r="A365" s="0" t="str">
-        <v>2026-02-21</v>
+        <v>2026-03-01</v>
       </c>
     </row>
     <row r="366" spans="1:1" customFormat="false">
       <c r="A366" s="0" t="str">
-        <v>2026-02-22</v>
+        <v>2026-03-02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>